<commit_message>
modified framework with winnium desktop scripts
</commit_message>
<xml_diff>
--- a/data/NewESRIHomePage.xlsx
+++ b/data/NewESRIHomePage.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\ESRI_TEST\ESRI-SEL-Auto\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESRI_Automation\IAM_Project\ESRI-SElenium-FW\ESRI_Sel_POM_Framework\com.esri.test.automation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="141"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="111">
+  <si>
+    <t>EsriAccountsUrl</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>SignInBtn</t>
+  </si>
   <si>
     <t>NewEsriSiteCoreURL</t>
   </si>
@@ -27,47 +39,328 @@
     <t>Image1Header</t>
   </si>
   <si>
-    <t>ArcGIS Imagery Basemap Update 2016</t>
-  </si>
-  <si>
-    <t>Port of Los Angeles Delivers Faster with ArcGIS</t>
-  </si>
-  <si>
-    <t>http://uat.esri.com/newhome</t>
+    <t>Image1Link</t>
+  </si>
+  <si>
+    <t>Image2Btn</t>
   </si>
   <si>
     <t>Image2Header</t>
   </si>
   <si>
+    <t>Image2Link</t>
+  </si>
+  <si>
+    <t>Image3Btn</t>
+  </si>
+  <si>
     <t>Image3Header</t>
   </si>
   <si>
+    <t>Image3Link</t>
+  </si>
+  <si>
+    <t>Image4Btn</t>
+  </si>
+  <si>
     <t>Image4Header</t>
   </si>
   <si>
+    <t>Image4Link</t>
+  </si>
+  <si>
+    <t>Quote1Btn</t>
+  </si>
+  <si>
     <t>Quote1</t>
   </si>
   <si>
-    <t>Esri products are so versatile that they have been used to combat deadly viruses, thwart terrorism, clean up environmental disasters and cheat at Pokémon Go</t>
+    <t>Quote2Btn</t>
   </si>
   <si>
     <t>Quote2</t>
   </si>
   <si>
+    <t>Quote3Btn</t>
+  </si>
+  <si>
     <t>Quote3</t>
   </si>
   <si>
-    <t>The holy grail of mapping toolboxes may reside with Esri.</t>
-  </si>
-  <si>
-    <t>Another grail of mapping toolboxes may also reside with Irse. Just sayin’.</t>
+    <t>AboutESRIHeader</t>
+  </si>
+  <si>
+    <t>LocationStrategyHeader</t>
+  </si>
+  <si>
+    <t>DevSummitHeader</t>
+  </si>
+  <si>
+    <t>GeoAppsHeader</t>
+  </si>
+  <si>
+    <t>ArcGISLink</t>
+  </si>
+  <si>
+    <t>ProdHignLigLink</t>
+  </si>
+  <si>
+    <t>ProdHignLigImg</t>
+  </si>
+  <si>
+    <t>IndustryLink</t>
+  </si>
+  <si>
+    <t>IndIniLink</t>
+  </si>
+  <si>
+    <t>IndIniImg</t>
+  </si>
+  <si>
+    <t>NewsLink</t>
+  </si>
+  <si>
+    <t>LatNewsLink</t>
+  </si>
+  <si>
+    <t>LatNewsImg</t>
+  </si>
+  <si>
+    <t>EventsLink</t>
+  </si>
+  <si>
+    <t>UpEventsLink</t>
+  </si>
+  <si>
+    <t>UpEventsImg</t>
+  </si>
+  <si>
+    <t>MapWeLoveLink</t>
+  </si>
+  <si>
+    <t>FeaturedMapLink</t>
+  </si>
+  <si>
+    <t>FeaturedMapImg</t>
+  </si>
+  <si>
+    <t>AboutESRILink</t>
+  </si>
+  <si>
+    <t>WhatsGISLink</t>
+  </si>
+  <si>
+    <t>EsriHomeLink</t>
+  </si>
+  <si>
+    <t>EventsHeader</t>
+  </si>
+  <si>
+    <t>userconferenceHeader</t>
+  </si>
+  <si>
+    <t>MapsWeLoveHeader</t>
+  </si>
+  <si>
+    <t>MinneapolisSolarHeader</t>
+  </si>
+  <si>
+    <t>EmailBtn</t>
+  </si>
+  <si>
+    <t>InstaBtn</t>
+  </si>
+  <si>
+    <t>TwitterBtn</t>
+  </si>
+  <si>
+    <t>FbBtn</t>
+  </si>
+  <si>
+    <t>LinkedInBtn</t>
+  </si>
+  <si>
+    <t>GooglePlusBtn</t>
+  </si>
+  <si>
+    <t>RssBtn</t>
+  </si>
+  <si>
+    <t>IndustriesHeader</t>
+  </si>
+  <si>
+    <t>OperationalIntelligenceHeader</t>
+  </si>
+  <si>
+    <t>https://accounts.esri.com/?redirect_uri=http://www.esri.com/</t>
+  </si>
+  <si>
+    <t>trainingTest1</t>
+  </si>
+  <si>
+    <t>Test1234</t>
+  </si>
+  <si>
+    <t>SignIn</t>
+  </si>
+  <si>
+    <t>http://uat.esri.com</t>
+  </si>
+  <si>
+    <t>Unlock the Full Potential of Your Data</t>
+  </si>
+  <si>
+    <t>See how with The Science Of Where</t>
+  </si>
+  <si>
+    <t>Location Strategy for Business</t>
+  </si>
+  <si>
+    <t>Uncover actionable insights</t>
+  </si>
+  <si>
+    <t>Esri Developer Summit</t>
+  </si>
+  <si>
+    <t>Experience the Next Generation of GIS</t>
+  </si>
+  <si>
+    <t>Test drive new technology at DevSummit</t>
+  </si>
+  <si>
+    <t>Do-It-Yourself Geo Apps</t>
+  </si>
+  <si>
+    <t>Register for a free online course</t>
+  </si>
+  <si>
+    <t>Quote 1</t>
+  </si>
+  <si>
+    <t>Esri products are so versatile that they have been used to combat deadly viruses, thwart terrorism, clean up environmental disasters and cheat at Pokémon Go.</t>
+  </si>
+  <si>
+    <t>Quote 2</t>
+  </si>
+  <si>
+    <t>[Esri has] some of the most extensive capabilities for capturing spatial data and the analyses, presentation, and delivery of spatial insights.</t>
+  </si>
+  <si>
+    <t>Quote 3</t>
+  </si>
+  <si>
+    <t>Data meets geography at Esri, a billion-dollar company whose mapping technology enables feats like predicting flash floods, managing supply chains in real time, and cutting disease outbreaks off at the pass.</t>
+  </si>
+  <si>
+    <t>We pioneer problem solving using GIS</t>
+  </si>
+  <si>
+    <t>Location Strategy For Business</t>
+  </si>
+  <si>
+    <t>Esri Developer
+Summit</t>
+  </si>
+  <si>
+    <t>Do-It-Yourself
+Geo Apps</t>
+  </si>
+  <si>
+    <t>ArcGIS</t>
+  </si>
+  <si>
+    <t>Production Spotlight</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Industry Initiative</t>
+  </si>
+  <si>
+    <t>Latest News</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Upcoming Events</t>
+  </si>
+  <si>
+    <t>Maps We Love</t>
+  </si>
+  <si>
+    <t>Featured Map</t>
+  </si>
+  <si>
+    <t>About ESRI</t>
+  </si>
+  <si>
+    <t>What is GIS</t>
+  </si>
+  <si>
+    <t>Esri Home</t>
+  </si>
+  <si>
+    <t>Esri User Conference</t>
+  </si>
+  <si>
+    <t>Explore. Learn. Be Inspired.</t>
+  </si>
+  <si>
+    <t>Minneapolis Solar Suitability</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Google Plus</t>
+  </si>
+  <si>
+    <t>Rss-News Feed</t>
+  </si>
+  <si>
+    <t>ESRINewsHeader</t>
+  </si>
+  <si>
+    <t>GIS_IONHeader</t>
+  </si>
+  <si>
+    <t>Industries</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Making Better Operational Decisions</t>
+  </si>
+  <si>
+    <t>GIS: Improving Our Nation and Public Sector Decisions</t>
+  </si>
+  <si>
+    <t>ArcGISWhatsNewHeader</t>
+  </si>
+  <si>
+    <t>What's New</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,13 +372,6 @@
       <color rgb="FF6A3E3E"/>
       <name val="Courier New"/>
       <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF6A3E3E"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -123,14 +409,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -293,6 +587,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -328,6 +639,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -480,86 +808,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFFFFF"/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:BH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BH5" sqref="BH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375"/>
-    <col min="2" max="2" width="35.140625"/>
-    <col min="3" max="3" width="48"/>
-    <col min="4" max="4" width="46"/>
-    <col min="5" max="5" width="48"/>
-    <col min="6" max="970" width="11.5703125"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:60" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
+    <row r="2" spans="1:60" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
+        <v>60</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>13</v>
+        <v>64</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="BH2" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added ETC test and generic wrappers methods
</commit_message>
<xml_diff>
--- a/data/NewESRIHomePage.xlsx
+++ b/data/NewESRIHomePage.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESRI_Automation\IAM_Project\ESRI-SElenium-FW\ESRI_Sel_POM_Framework\com.esri.test.automation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\ESRI_TEST\ESRI-SEL-Auto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="111">
   <si>
     <t>EsriAccountsUrl</t>
   </si>
@@ -354,41 +354,6 @@
   </si>
   <si>
     <t>What's New</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="//www.googletagmanager.com/ns.html?id=GTM-WFJ52X"
-height="0" width="0" style="display:none;visibility:hidden"&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>GoogleTagManagerNoScript</t>
-  </si>
-  <si>
-    <t>GoogleTagManagerScript</t>
-  </si>
-  <si>
-    <t>HeaderEmbedCode</t>
-  </si>
-  <si>
-    <t>FooterEmbedCode</t>
-  </si>
-  <si>
-    <t>PardotLayerCode</t>
-  </si>
-  <si>
-    <t>(function(w,d,s,l,i){w[l]=w[l]||[];w[l].push({'gtm.start':
-new Date().getTime(),event:'gtm.js'});var f=d.getElementsByTagName(s)[0],
-j=d.createElement(s),dl=l!='dataLayer'?'&amp;l='+l:'';j.async=true;j.src=
-'//www.googletagmanager.com/gtm.js?id='+i+dl;f.parentNode.insertBefore(j,f);
-})(window,document,'script','dataLayer','GTM-WFJ52X');</t>
-  </si>
-  <si>
-    <t>http://assets.adobedtm.com/2e9cd01e19dc5ac4867e752f17a2f1ea1923e5af/satelliteLib-0ed1001fd441a838aefe8e755be42aaafddcc46b.js</t>
-  </si>
-  <si>
-    <t>_satellite.pageBottom();</t>
-  </si>
-  <si>
-    <t>http://go.pardot.com/dcjs/82202/1182/dc.js</t>
   </si>
 </sst>
 </file>
@@ -446,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -460,10 +425,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -626,23 +587,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -678,23 +622,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -847,19 +774,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM2"/>
+  <dimension ref="A1:BH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
-      <selection activeCell="BI9" sqref="BI9"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BI1" sqref="BI1:BN1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="61" max="61" width="72.140625" customWidth="1"/>
-    <col min="62" max="62" width="72" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:60" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1040,23 +963,8 @@
       <c r="BH1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BI1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>116</v>
-      </c>
     </row>
-    <row r="2" spans="1:65" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -1236,21 +1144,6 @@
       </c>
       <c r="BH2" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="BI2" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="BJ2" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="BK2" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>119</v>
-      </c>
-      <c r="BM2" s="6" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>